<commit_message>
Added shell for tests that push to GitHub
</commit_message>
<xml_diff>
--- a/demo/demo_grades.xlsx
+++ b/demo/demo_grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Code/AltGradebook/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Code/AltGradebook/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840124AA-EE9E-6D47-BF92-7BEC79AA7D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939E40DD-2FED-A84A-9517-2AE5A80CE325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="500" windowWidth="28500" windowHeight="17600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38100" yWindow="2180" windowWidth="28500" windowHeight="17600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="131">
   <si>
     <t>Last Name</t>
   </si>
@@ -420,16 +420,30 @@
   </si>
   <si>
     <t>mxx</t>
+  </si>
+  <si>
+    <t>Implement CSS</t>
+  </si>
+  <si>
+    <t>ExpressJS</t>
+  </si>
+  <si>
+    <t>xjs1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -452,8 +466,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1445,7 +1460,7 @@
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="str">
         <f>info!A1</f>
         <v>Last Name</v>
@@ -1477,8 +1492,14 @@
       <c r="I1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>lname</v>
@@ -1513,8 +1534,11 @@
       <c r="J2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K2" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Bright</v>
@@ -1546,8 +1570,11 @@
       <c r="I3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Dean</v>
@@ -1579,8 +1606,11 @@
       <c r="I4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Flowers</v>
@@ -1612,8 +1642,11 @@
       <c r="I5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Frank</v>
@@ -1646,7 +1679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Henry</v>
@@ -1679,7 +1712,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Howel</v>
@@ -1711,8 +1744,11 @@
       <c r="I8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>Jacobs</v>
@@ -1745,7 +1781,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>Jackson</v>
@@ -1778,7 +1814,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>King</v>
@@ -1811,7 +1847,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Klein</v>
@@ -1844,7 +1880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Lowery</v>
@@ -1877,7 +1913,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
         <f>info!A14</f>
         <v>Mckinney</v>
@@ -1910,7 +1946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
         <f>info!A15</f>
         <v>Mills</v>
@@ -1943,7 +1979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
         <f>info!A16</f>
         <v>Morrison</v>
@@ -1976,7 +2012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f>info!A17</f>
         <v>Nguyen</v>
@@ -2009,7 +2045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f>info!A18</f>
         <v>Noraburta</v>
@@ -2042,7 +2078,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f>info!A19</f>
         <v>Nunez</v>
@@ -2075,7 +2111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f>info!A20</f>
         <v>Patterson</v>
@@ -2108,7 +2144,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f>info!A21</f>
         <v>Poole</v>
@@ -2141,7 +2177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f>info!A22</f>
         <v>Phillips</v>
@@ -2174,7 +2210,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>info!A23</f>
         <v>Shearman</v>
@@ -2195,7 +2231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f>info!A24</f>
         <v>Spears</v>
@@ -2228,7 +2264,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f>info!A25</f>
         <v>Tate</v>
@@ -2260,8 +2296,11 @@
       <c r="I25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" t="str">
         <f>info!A26</f>
         <v>Taylor</v>
@@ -2293,8 +2332,11 @@
       <c r="I26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" t="str">
         <f>info!A27</f>
         <v>Waterson</v>
@@ -2327,7 +2369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" t="str">
         <f>info!A28</f>
         <v>Zyer</v>
@@ -3886,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91792C2-488C-3549-A3D4-732CA45379CB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3934,6 +3976,9 @@
         <f>info!E3</f>
         <v>brightw</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
@@ -3973,6 +4018,9 @@
         <f>info!E5</f>
         <v>flowersj</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="str">
@@ -3991,6 +4039,9 @@
         <f>info!E6</f>
         <v>frankc</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="str">
@@ -4030,6 +4081,9 @@
         <f>info!E8</f>
         <v>howelh</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="str">
@@ -4132,6 +4186,9 @@
         <f>info!E13</f>
         <v>loweryn</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
@@ -4192,6 +4249,9 @@
         <f>info!E16</f>
         <v>morrisonr</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
@@ -4210,6 +4270,9 @@
         <f>info!E17</f>
         <v>nguyenb</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
@@ -4249,6 +4312,9 @@
         <f>info!E19</f>
         <v>nunezs</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
@@ -4267,6 +4333,9 @@
         <f>info!E20</f>
         <v>pattersonl</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
@@ -4285,6 +4354,9 @@
         <f>info!E21</f>
         <v>poolem</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
@@ -4303,6 +4375,9 @@
         <f>info!E22</f>
         <v>phillipsr</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
@@ -4321,6 +4396,9 @@
         <f>info!E23</f>
         <v>shearmanc</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
@@ -4360,6 +4438,9 @@
         <f>info!E25</f>
         <v>tatea</v>
       </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
@@ -4399,6 +4480,9 @@
         <f>info!E27</f>
         <v>watersonw</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="str">

</xml_diff>

<commit_message>
It works\! Can specify base output directory and it's passed to the JS image generator
</commit_message>
<xml_diff>
--- a/demo/demo_grades.xlsx
+++ b/demo/demo_grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Code/AltGradebook/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939E40DD-2FED-A84A-9517-2AE5A80CE325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B432E302-8F5D-EA45-BB0C-681EB60C0458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38100" yWindow="2180" windowWidth="28500" windowHeight="17600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="1200" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -329,9 +329,6 @@
     <t>Spears</t>
   </si>
   <si>
-    <t>Shearman</t>
-  </si>
-  <si>
     <t>Tate</t>
   </si>
   <si>
@@ -429,6 +426,9 @@
   </si>
   <si>
     <t>xjs1</t>
+  </si>
+  <si>
+    <t>xxShearman</t>
   </si>
 </sst>
 </file>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E28"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -909,7 +909,7 @@
         <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -931,7 +931,7 @@
         <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -953,7 +953,7 @@
         <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -997,7 +997,7 @@
         <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -1063,7 +1063,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1129,7 +1129,7 @@
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1173,7 +1173,7 @@
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -1195,7 +1195,7 @@
         <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -1217,7 +1217,7 @@
         <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -1261,7 +1261,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -1301,22 +1301,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>97</v>
+      <c r="A23" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>shearmanc</v>
+        <v>xxshearmanc</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>shearmanc</v>
+        <v>xxshearmanc</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1390,10 +1390,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -1452,7 +1452,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1493,10 +1493,10 @@
         <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -1535,7 +1535,7 @@
         <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
@@ -1835,7 +1835,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
         <v>67</v>
@@ -1898,19 +1898,19 @@
         <v>loweryn</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G13" t="s">
         <v>65</v>
       </c>
       <c r="H13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" t="s">
         <v>125</v>
-      </c>
-      <c r="I13" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -2000,7 +2000,7 @@
         <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
@@ -2033,7 +2033,7 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -2099,7 +2099,7 @@
         <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
@@ -2132,7 +2132,7 @@
         <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
         <v>67</v>
@@ -2210,10 +2210,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>info!A23</f>
-        <v>Shearman</v>
+        <v>xxShearman</v>
       </c>
       <c r="B23" t="str">
         <f>info!B23</f>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="D23" t="str">
         <f>info!E23</f>
-        <v>shearmanc</v>
+        <v>xxshearmanc</v>
       </c>
       <c r="E23" t="s">
         <v>22</v>
@@ -2435,7 +2435,7 @@
         <v>GitHub</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -2456,7 +2456,7 @@
         <v>github</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -2561,7 +2561,7 @@
         <v>henryd</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2750,7 +2750,7 @@
         <v>morrisonr</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -2813,7 +2813,7 @@
         <v>nunezs</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -2834,7 +2834,7 @@
         <v>pattersonl</v>
       </c>
       <c r="E20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -2882,7 +2882,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>info!A23</f>
-        <v>Shearman</v>
+        <v>xxShearman</v>
       </c>
       <c r="B23" t="str">
         <f>info!B23</f>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="D23" t="str">
         <f>info!E23</f>
-        <v>shearmanc</v>
+        <v>xxshearmanc</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
@@ -3745,7 +3745,7 @@
     <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>info!A23</f>
-        <v>Shearman</v>
+        <v>xxShearman</v>
       </c>
       <c r="B23" t="str">
         <f>info!B23</f>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="D23" t="str">
         <f>info!E23</f>
-        <v>shearmanc</v>
+        <v>xxshearmanc</v>
       </c>
       <c r="E23" t="s">
         <v>24</v>
@@ -3928,7 +3928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91792C2-488C-3549-A3D4-732CA45379CB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -4382,7 +4382,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f>info!A23</f>
-        <v>Shearman</v>
+        <v>xxShearman</v>
       </c>
       <c r="B22" t="str">
         <f>info!B23</f>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="D22" t="str">
         <f>info!E23</f>
-        <v>shearmanc</v>
+        <v>xxshearmanc</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Fix bug in handling of blank columns
</commit_message>
<xml_diff>
--- a/demo/demo_grades.xlsx
+++ b/demo/demo_grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Code/AltGradebook/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B432E302-8F5D-EA45-BB0C-681EB60C0458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3128A670-D677-6E48-865B-30FE61B8910A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="1200" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="132">
   <si>
     <t>Last Name</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>xxShearman</t>
+  </si>
+  <si>
+    <t>ex</t>
   </si>
 </sst>
 </file>
@@ -808,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1452,7 +1455,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3928,8 +3931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91792C2-488C-3549-A3D4-732CA45379CB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4481,7 +4484,7 @@
         <v>watersonw</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>